<commit_message>
Adicionando tabela à documentação
</commit_message>
<xml_diff>
--- a/Modelagem/SP Medical Group - Modelagem Lógica.xlsx
+++ b/Modelagem/SP Medical Group - Modelagem Lógica.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Modelagem Lógica" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -159,7 +159,43 @@
     <t>Adiado</t>
   </si>
   <si>
-    <t>Só tem mais 10 dias de vida.</t>
+    <t>Cláudia Joaquina</t>
+  </si>
+  <si>
+    <t>claudia22@email.com</t>
+  </si>
+  <si>
+    <t>Foi receitado medimento x...</t>
+  </si>
+  <si>
+    <t>Precisa ser medicado diariamente.</t>
+  </si>
+  <si>
+    <t>(11) 94444-4444</t>
+  </si>
+  <si>
+    <t>(11) 95555-5555</t>
+  </si>
+  <si>
+    <t>(11) 96666-6666</t>
+  </si>
+  <si>
+    <t>(11) 97777-7777</t>
+  </si>
+  <si>
+    <t>(11) 9888-88888</t>
+  </si>
+  <si>
+    <t>123.123.113-23</t>
+  </si>
+  <si>
+    <t>234.235.523-24</t>
+  </si>
+  <si>
+    <t>12.123.123-1</t>
+  </si>
+  <si>
+    <t>45.456.234-9</t>
   </si>
 </sst>
 </file>
@@ -210,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -270,12 +306,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,21 +353,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -591,97 +659,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection sqref="A1:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="7"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
@@ -695,38 +727,14 @@
       <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2">
-        <v>11944444444</v>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>3</v>
-      </c>
-      <c r="L3" s="2">
-        <v>121231231</v>
-      </c>
-      <c r="M3" s="2">
-        <v>12312311323</v>
-      </c>
-      <c r="N3" s="4">
-        <v>36537</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
@@ -740,38 +748,20 @@
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2">
-        <v>11955555555</v>
+      <c r="D4" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>4</v>
-      </c>
-      <c r="L4" s="2">
-        <v>454562349</v>
-      </c>
-      <c r="M4" s="2">
-        <v>23423552324</v>
-      </c>
-      <c r="N4" s="4">
-        <v>16526</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
@@ -785,26 +775,20 @@
       <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2">
-        <v>11966666666</v>
+      <c r="D5" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="2">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
@@ -818,8 +802,8 @@
       <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="2">
-        <v>11977777777</v>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E6" s="2">
         <v>3</v>
@@ -828,31 +812,41 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
@@ -866,12 +860,12 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
@@ -885,12 +879,12 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
@@ -898,53 +892,53 @@
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="9"/>
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="11"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
@@ -966,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -980,16 +974,24 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="12">
+        <v>2</v>
+      </c>
+      <c r="B13" s="12">
+        <v>5</v>
+      </c>
+      <c r="C13" s="12">
+        <v>4</v>
+      </c>
+      <c r="D13" s="12">
+        <v>9812739918</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1003,198 +1005,311 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="H16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2">
-        <v>4</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="L16" s="4">
-        <v>43567</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16" s="2">
-        <v>2</v>
-      </c>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="E19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="B27" s="2">
         <v>3</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="C27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="4">
+        <v>36537</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="4">
+        <v>16526</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>43567</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="12">
+        <v>2</v>
+      </c>
+      <c r="B34" s="12">
+        <v>2</v>
+      </c>
+      <c r="C34" s="12">
+        <v>1</v>
+      </c>
+      <c r="D34" s="14">
+        <v>43621</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="I14:N14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C5" r:id="rId3"/>
     <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>